<commit_message>
Models can be filled with data (except for arrays)
Allow Model containers to load models
Models can be filled with data
3 types of models
Direct: values are put into the model directly
List and dictionary
Updated excel file with data
</commit_message>
<xml_diff>
--- a/ExcelFiles/Excel_DB.xlsx
+++ b/ExcelFiles/Excel_DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\AtDb\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1073AA7B-891A-4754-811D-1B5BE318F07B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BAF682-5BA5-4E31-B5A0-1AF1660E288F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{423AF900-AA07-4388-B93C-A3173C320567}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{423AF900-AA07-4388-B93C-A3173C320567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,29 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
-  <si>
-    <t xml:space="preserve"> @@TableName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t xml:space="preserve"> @@End</t>
   </si>
   <si>
-    <t xml:space="preserve"> @@OtherTable</t>
-  </si>
-  <si>
-    <t>uid</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -60,31 +48,169 @@
     <t>d</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>bool_2</t>
-  </si>
-  <si>
-    <t>bool_1</t>
-  </si>
-  <si>
-    <t>bool_0</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>Ling</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>{"Encrypted":true,"Export":true,"LookupTable":true,"IntermediateTable":false}</t>
+    <t xml:space="preserve"> @@People</t>
+  </si>
+  <si>
+    <t>words</t>
+  </si>
+  <si>
+    <t>string_0</t>
+  </si>
+  <si>
+    <t>string_1</t>
+  </si>
+  <si>
+    <t>string_2</t>
+  </si>
+  <si>
+    <t>string_3</t>
+  </si>
+  <si>
+    <t>these</t>
+  </si>
+  <si>
+    <t>tony</t>
+  </si>
+  <si>
+    <t>stark</t>
+  </si>
+  <si>
+    <t>steve</t>
+  </si>
+  <si>
+    <t>rogers</t>
+  </si>
+  <si>
+    <t>bruce</t>
+  </si>
+  <si>
+    <t>banner</t>
+  </si>
+  <si>
+    <t>nick</t>
+  </si>
+  <si>
+    <t>fury</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>iron</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
+  <si>
+    <t>mo</t>
+  </si>
+  <si>
+    <t>ther</t>
+  </si>
+  <si>
+    <t>f*</t>
+  </si>
+  <si>
+    <t>cker</t>
+  </si>
+  <si>
+    <t>{"TableName":"People","ClassName":"People","Encrypted":true,"Export":true,"Style":2}</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>string_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @@ListObject</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @@DirectObject</t>
+  </si>
+  <si>
+    <t>{"TableName":"DirectObject","ClassName":"DirectObject","Encrypted":true,"Export":true,"Style":0}</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>is a</t>
+  </si>
+  <si>
+    <t>settings file</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @@end</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @aBool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @aInt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @aFloat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @aString</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @stringArray</t>
+  </si>
+  <si>
+    <t>ignoredValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @uid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @age</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @words</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @firstSetting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @secondSetting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @thirdSetting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @floatValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @intValue</t>
+  </si>
+  <si>
+    <t>{"TableName":"ListObject","ClassName":"ListFile","Encrypted":true,"Export":true,"Style":1}</t>
   </si>
 </sst>
 </file>
@@ -436,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6ABFAC-7C07-43B6-99A9-C97CC8759C12}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,160 +573,384 @@
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>-100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B13">
+        <v>200</v>
+      </c>
+      <c r="C13">
+        <v>-200</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+      <c r="H13">
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix arrays not being filled
Changed how arrays are constructed
filled arrays with data
</commit_message>
<xml_diff>
--- a/ExcelFiles/Excel_DB.xlsx
+++ b/ExcelFiles/Excel_DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\AtDb\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BAF682-5BA5-4E31-B5A0-1AF1660E288F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F81FC9B-0362-48BC-AE9B-E1B00040C334}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{423AF900-AA07-4388-B93C-A3173C320567}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t xml:space="preserve"> @@End</t>
   </si>
@@ -138,9 +138,6 @@
     <t>two</t>
   </si>
   <si>
-    <t>string_4</t>
-  </si>
-  <si>
     <t xml:space="preserve"> @@ListObject</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t xml:space="preserve"> @aString</t>
   </si>
   <si>
-    <t xml:space="preserve"> @stringArray</t>
-  </si>
-  <si>
     <t>ignoredValue</t>
   </si>
   <si>
@@ -211,6 +205,24 @@
   </si>
   <si>
     <t>{"TableName":"ListObject","ClassName":"ListFile","Encrypted":true,"Export":true,"Style":1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @intArray</t>
+  </si>
+  <si>
+    <t>int_0</t>
+  </si>
+  <si>
+    <t>int_1</t>
+  </si>
+  <si>
+    <t>int_2</t>
+  </si>
+  <si>
+    <t>int_3</t>
+  </si>
+  <si>
+    <t>int_4</t>
   </si>
 </sst>
 </file>
@@ -564,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6ABFAC-7C07-43B6-99A9-C97CC8759C12}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,29 +587,29 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>56</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -619,13 +631,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -636,49 +648,49 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" t="s">
         <v>48</v>
-      </c>
-      <c r="E10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -695,19 +707,19 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="J11" t="s">
         <v>1</v>
@@ -794,28 +806,28 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>53</v>
       </c>
-      <c r="D18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Flagged enum support
</commit_message>
<xml_diff>
--- a/ExcelFiles/Excel_DB.xlsx
+++ b/ExcelFiles/Excel_DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\AtDb\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DC447E-8E42-44DB-8E77-9A5EC9CE7799}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A2880C-5884-4703-A44B-BB13EF6E4BCA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{423AF900-AA07-4388-B93C-A3173C320567}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
   <si>
     <t xml:space="preserve"> @@End</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t xml:space="preserve"> @OtherEnum</t>
+  </si>
+  <si>
+    <t>flagged</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1015,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1041,7 @@
         <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added composite enum support
Refactored how enums are generated
3 types: normal, flagged, composite
</commit_message>
<xml_diff>
--- a/ExcelFiles/Excel_DB.xlsx
+++ b/ExcelFiles/Excel_DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\AtDb\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A2880C-5884-4703-A44B-BB13EF6E4BCA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88F8A65-CB3B-42D6-8718-94E1F9E7547C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{423AF900-AA07-4388-B93C-A3173C320567}"/>
+    <workbookView xWindow="-525" yWindow="660" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{423AF900-AA07-4388-B93C-A3173C320567}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
   <si>
     <t xml:space="preserve"> @@End</t>
   </si>
@@ -256,23 +256,71 @@
     <t xml:space="preserve"> @MyEnum</t>
   </si>
   <si>
-    <t>enum</t>
-  </si>
-  <si>
     <t xml:space="preserve"> @OtherEnum</t>
   </si>
   <si>
-    <t>flagged</t>
+    <t xml:space="preserve"> @FlagsTest</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Flagged</t>
+  </si>
+  <si>
+    <t>Composite</t>
+  </si>
+  <si>
+    <t>None, 0</t>
+  </si>
+  <si>
+    <t>Ground, 1</t>
+  </si>
+  <si>
+    <t>Road, &lt;&lt;1, //DO NOT USE DIRECTLY</t>
+  </si>
+  <si>
+    <t>Road2Lane, Road, &lt;&lt;2</t>
+  </si>
+  <si>
+    <t>Road4Lane, Road, &lt;&lt;3</t>
+  </si>
+  <si>
+    <t>RoadBus, Road, &lt;&lt;4</t>
+  </si>
+  <si>
+    <t>Road6Lane, Road, &lt;&lt;5</t>
+  </si>
+  <si>
+    <t>RoadTram, Road, &lt;&lt;6</t>
+  </si>
+  <si>
+    <t>Rail, &lt;&lt;7</t>
+  </si>
+  <si>
+    <t>Invalid, &lt;&lt;8</t>
+  </si>
+  <si>
+    <t>Road2LaneTo4Lane, Road2Lane,Road4Lane</t>
+  </si>
+  <si>
+    <t>AllInfrastructure, Road2Lane,Road4Lane,Road6Lane,RoadBus,RoadTram,Rail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1012,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5272D9B9-1E90-457D-84C2-55BBA9BF6005}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,67 +1071,124 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>75</v>
       </c>
       <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
       <c r="B6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>